<commit_message>
Team3_Product Backlog - User Stories
</commit_message>
<xml_diff>
--- a/03-Documentation/Team3_Product Backlog-Matrix_frame_work_HU.xlsx
+++ b/03-Documentation/Team3_Product Backlog-Matrix_frame_work_HU.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\SEPTIMO\Team3DevSolutions\03-Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203F448A-473D-49C4-B412-EDE859BFDB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68D491B-DF3F-413E-8ED6-75A6446E3FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>ITEM</t>
   </si>
@@ -136,39 +136,15 @@
     <t>Add Prodcuts</t>
   </si>
   <si>
-    <t>Add Users</t>
-  </si>
-  <si>
-    <t>List Products</t>
-  </si>
-  <si>
-    <t>List Users</t>
-  </si>
-  <si>
     <t>Product entry is required</t>
   </si>
   <si>
-    <t>See the products</t>
-  </si>
-  <si>
-    <t>See the users</t>
-  </si>
-  <si>
-    <t>Adding users is required</t>
-  </si>
-  <si>
     <t>Registration of products in inventory</t>
   </si>
   <si>
     <t>Review inventory products</t>
   </si>
   <si>
-    <t>User registration in the system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rerview the users registred in the system </t>
-  </si>
-  <si>
     <t>Administrator</t>
   </si>
   <si>
@@ -178,9 +154,6 @@
     <t>Enter the product list module, click enter, the application displays the list of stored products</t>
   </si>
   <si>
-    <t>Enter the user list module, click enter, the application displays the list of stored users</t>
-  </si>
-  <si>
     <t>Mateo Loachamin</t>
   </si>
   <si>
@@ -190,15 +163,9 @@
     <t>The interface shows the screen to add products</t>
   </si>
   <si>
-    <t>The interface shows the screen to add users</t>
-  </si>
-  <si>
     <t>The interface shows the added products</t>
   </si>
   <si>
-    <t>The interface shows the added users</t>
-  </si>
-  <si>
     <t>It is necessary that the system allows to correctly add the data to the database</t>
   </si>
   <si>
@@ -208,15 +175,9 @@
     <t>Add Products  to the system</t>
   </si>
   <si>
-    <t xml:space="preserve">Add Users to the system </t>
-  </si>
-  <si>
     <t>List Products to the system</t>
   </si>
   <si>
-    <t>List Users to the system</t>
-  </si>
-  <si>
     <t>USERNAME</t>
   </si>
   <si>
@@ -238,34 +199,55 @@
     <t>USER STORIES (HU) iSoftware.ec</t>
   </si>
   <si>
-    <t>REQ005</t>
-  </si>
-  <si>
-    <t>It is required to determine the business rules</t>
-  </si>
-  <si>
-    <t>Perform calculations for each business</t>
-  </si>
-  <si>
-    <t>Whe entering the products, the system performs the calculation of: Calculation of distributed price, calcularion of VAT, unit profit, total profit, customer discount</t>
-  </si>
-  <si>
-    <t>All teams</t>
-  </si>
-  <si>
-    <t>It is verified by entering to see the list of added products</t>
-  </si>
-  <si>
-    <t>Its is recommended to validate that the operations are correct</t>
-  </si>
-  <si>
     <t>Product Backlog - Matrix frame of work HU</t>
   </si>
   <si>
-    <t>Implement business rules</t>
-  </si>
-  <si>
-    <t>Implement business rules in the application</t>
+    <t>update Products</t>
+  </si>
+  <si>
+    <t>List Inventory</t>
+  </si>
+  <si>
+    <t>delete Products</t>
+  </si>
+  <si>
+    <t>Allow to delete products</t>
+  </si>
+  <si>
+    <t>Let me update the inventory information</t>
+  </si>
+  <si>
+    <t>Remove items from inventory</t>
+  </si>
+  <si>
+    <t>Inventory listing requiered</t>
+  </si>
+  <si>
+    <t>Product infromation needs to updated</t>
+  </si>
+  <si>
+    <t>Inventory is entered, product edit is clicked, data is update, information is saved</t>
+  </si>
+  <si>
+    <t>The inventory is entered, the product to be eliminated is chosen, the product to be eliminated is clicked, the system redirtects to the index</t>
+  </si>
+  <si>
+    <t>The interface shows the screen to update products</t>
+  </si>
+  <si>
+    <t>The interface remove the products</t>
+  </si>
+  <si>
+    <t>It is necessary that the system update correctly to the database</t>
+  </si>
+  <si>
+    <t>It is required to verify that the information, has been remove the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update Products to the system </t>
+  </si>
+  <si>
+    <t>Eliminar Products to the system</t>
   </si>
 </sst>
 </file>
@@ -790,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -870,6 +852,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -879,6 +879,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -905,6 +916,44 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -914,76 +963,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1296,10 +1275,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q988"/>
+  <dimension ref="B1:Q987"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1334,22 +1313,22 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="2:17" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
+      <c r="B3" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="G4" s="4"/>
@@ -1360,46 +1339,46 @@
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:17" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="F5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="74" t="s">
+      <c r="G5" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="74" t="s">
+      <c r="H5" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="74" t="s">
+      <c r="J5" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="74" t="s">
+      <c r="K5" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="74" t="s">
+      <c r="L5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="74" t="s">
+      <c r="M5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="76" t="s">
+      <c r="N5" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="74" t="s">
+      <c r="O5" s="40" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1408,22 +1387,22 @@
         <v>2</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I6" s="31">
         <v>2</v>
@@ -1437,40 +1416,40 @@
       <c r="L6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="72" t="s">
-        <v>48</v>
+      <c r="M6" s="39" t="s">
+        <v>39</v>
       </c>
       <c r="N6" s="36" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="O6" s="35" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" ht="57" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B7" s="31" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>73</v>
+        <v>59</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>54</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="30" t="s">
-        <v>69</v>
+        <v>34</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="I7" s="31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J7" s="32">
         <v>44882</v>
@@ -1478,17 +1457,17 @@
       <c r="K7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="31" t="s">
+      <c r="L7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="73" t="s">
-        <v>70</v>
-      </c>
-      <c r="N7" s="71" t="s">
-        <v>71</v>
+      <c r="M7" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="36" t="s">
+        <v>42</v>
       </c>
       <c r="O7" s="35" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="42.75" x14ac:dyDescent="0.2">
@@ -1496,22 +1475,22 @@
         <v>6</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>39</v>
+        <v>53</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>57</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="H8" s="31" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="I8" s="31">
         <v>2</v>
@@ -1522,40 +1501,40 @@
       <c r="K8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="36" t="s">
-        <v>53</v>
+      <c r="M8" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="N8" s="38" t="s">
+        <v>65</v>
       </c>
       <c r="O8" s="35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="71.25" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="57" x14ac:dyDescent="0.25">
       <c r="B9" s="31" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>62</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="I9" s="31">
         <v>2</v>
@@ -1569,73 +1548,35 @@
       <c r="L9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9" s="36" t="s">
-        <v>52</v>
+      <c r="M9" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="N9" s="38" t="s">
+        <v>66</v>
       </c>
       <c r="O9" s="35" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="31">
-        <v>2</v>
-      </c>
-      <c r="J10" s="32">
-        <v>44882</v>
-      </c>
-      <c r="K10" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="L10" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="M10" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="O10" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q10" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="Q9" s="6"/>
+    </row>
+    <row r="10" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="7"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G11" s="7"/>
+      <c r="E11" s="8"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="2"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="8"/>
+    <row r="12" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="2"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1644,10 +1585,10 @@
       <c r="K13" s="9"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="9"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="2:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1665,17 +1606,22 @@
     <row r="17" spans="9:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="3"/>
+      <c r="K17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="5"/>
     </row>
     <row r="18" spans="9:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="M18" s="5"/>
     </row>
@@ -1683,21 +1629,19 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="9:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="K20" s="2"/>
       <c r="L20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M20" s="5"/>
     </row>
@@ -1705,10 +1649,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M21" s="5"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22" spans="9:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="1"/>
@@ -1716,7 +1657,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="9:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="2"/>
@@ -2904,12 +2845,7 @@
       <c r="K220" s="2"/>
       <c r="L220" s="3"/>
     </row>
-    <row r="221" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I221" s="1"/>
-      <c r="J221" s="1"/>
-      <c r="K221" s="2"/>
-      <c r="L221" s="3"/>
-    </row>
+    <row r="221" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="222" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="223" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="224" spans="9:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3676,17 +3612,16 @@
     <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:O3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L6:L10" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>$L$18:$L$21</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L6:L9" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>$L$17:$L$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K6:K10" xr:uid="{00000000-0002-0000-0000-000001000000}">
-      <formula1>$K$18:$K$20</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K6:K9" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>$K$17:$K$19</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
@@ -3703,7 +3638,7 @@
   <dimension ref="B2:P1000"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3731,23 +3666,23 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="2:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="58"/>
+      <c r="B6" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="66"/>
     </row>
     <row r="7" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="11"/>
@@ -3787,15 +3722,15 @@
         <v>0</v>
       </c>
       <c r="D9" s="19"/>
-      <c r="E9" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="66"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="58"/>
+      <c r="I9" s="66"/>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
@@ -3807,20 +3742,20 @@
     <row r="10" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="17"/>
       <c r="C10" s="22" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="D10" s="23"/>
-      <c r="E10" s="59" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,5,0)</f>
+      <c r="E10" s="68" t="str">
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,5,0)</f>
         <v>Administrator</v>
       </c>
-      <c r="F10" s="58"/>
+      <c r="F10" s="66"/>
       <c r="G10" s="24"/>
-      <c r="H10" s="59" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,11,0)</f>
+      <c r="H10" s="68" t="str">
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,11,0)</f>
         <v>Terminado</v>
       </c>
-      <c r="I10" s="58"/>
+      <c r="I10" s="66"/>
       <c r="J10" s="24"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
@@ -3849,18 +3784,18 @@
     <row r="12" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="17"/>
       <c r="C12" s="18" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D12" s="23"/>
-      <c r="E12" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="58"/>
+      <c r="E12" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="66"/>
       <c r="G12" s="24"/>
-      <c r="H12" s="57" t="s">
+      <c r="H12" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="58"/>
+      <c r="I12" s="66"/>
       <c r="J12" s="24"/>
       <c r="K12" s="26"/>
       <c r="L12" s="26"/>
@@ -3872,21 +3807,21 @@
     <row r="13" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17"/>
       <c r="C13" s="22">
-        <f>VLOOKUP('User Stories'!C10,'Product Backlog- HU'!B6:O10,8,0)</f>
+        <f>VLOOKUP('User Stories'!C10,'Product Backlog- HU'!B6:O9,8,0)</f>
         <v>2</v>
       </c>
       <c r="D13" s="23"/>
-      <c r="E13" s="59" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,10,0)</f>
+      <c r="E13" s="68" t="str">
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,10,0)</f>
         <v>Alta</v>
       </c>
-      <c r="F13" s="58"/>
+      <c r="F13" s="66"/>
       <c r="G13" s="24"/>
-      <c r="H13" s="59" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,7,0)</f>
+      <c r="H13" s="68" t="str">
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,7,0)</f>
         <v>Ligia Maldonado</v>
       </c>
-      <c r="I13" s="58"/>
+      <c r="I13" s="66"/>
       <c r="J13" s="24"/>
       <c r="K13" s="26"/>
       <c r="L13" s="26"/>
@@ -3914,68 +3849,68 @@
     </row>
     <row r="15" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="17"/>
-      <c r="C15" s="39" t="s">
-        <v>61</v>
+      <c r="C15" s="45" t="s">
+        <v>48</v>
       </c>
       <c r="D15" s="69" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,3,0)</f>
-        <v>List Users</v>
-      </c>
-      <c r="E15" s="61"/>
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,3,0)</f>
+        <v>delete Products</v>
+      </c>
+      <c r="E15" s="49"/>
       <c r="F15" s="20"/>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="45" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="69" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,4,0)</f>
-        <v xml:space="preserve">Rerview the users registred in the system </v>
-      </c>
-      <c r="I15" s="77"/>
-      <c r="J15" s="78"/>
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,4,0)</f>
+        <v>Remove items from inventory</v>
+      </c>
+      <c r="I15" s="70"/>
+      <c r="J15" s="71"/>
       <c r="K15" s="20"/>
-      <c r="L15" s="39" t="s">
+      <c r="L15" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="M15" s="42" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,6,0)</f>
-        <v>Enter the user list module, click enter, the application displays the list of stored users</v>
-      </c>
-      <c r="N15" s="43"/>
-      <c r="O15" s="44"/>
+      <c r="M15" s="55" t="str">
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,6,0)</f>
+        <v>The inventory is entered, the product to be eliminated is chosen, the product to be eliminated is clicked, the system redirtects to the index</v>
+      </c>
+      <c r="N15" s="56"/>
+      <c r="O15" s="57"/>
       <c r="P15" s="21"/>
     </row>
     <row r="16" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="17"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="20"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="80"/>
-      <c r="J16" s="81"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="74"/>
       <c r="K16" s="20"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="47"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="60"/>
       <c r="P16" s="21"/>
     </row>
     <row r="17" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="17"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="63"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="84"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="76"/>
+      <c r="J17" s="77"/>
       <c r="K17" s="20"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="50"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="63"/>
       <c r="P17" s="21"/>
     </row>
     <row r="18" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3997,41 +3932,41 @@
     </row>
     <row r="19" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17"/>
-      <c r="C19" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="51" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,14,0)</f>
-        <v>List Users to the system</v>
-      </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="53"/>
+      <c r="C19" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="49"/>
+      <c r="E19" s="78" t="str">
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,14,0)</f>
+        <v>Eliminar Products to the system</v>
+      </c>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="80"/>
       <c r="P19" s="21"/>
     </row>
     <row r="20" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="17"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="56"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="82"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="82"/>
+      <c r="M20" s="82"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="83"/>
       <c r="P20" s="21"/>
     </row>
     <row r="21" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4053,63 +3988,63 @@
     </row>
     <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="17"/>
-      <c r="C22" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="42" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,12,0)</f>
-        <v>The interface shows the added users</v>
-      </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="44"/>
+      <c r="C22" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="55" t="str">
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,12,0)</f>
+        <v>The interface remove the products</v>
+      </c>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="57"/>
       <c r="I22" s="20"/>
-      <c r="J22" s="64" t="s">
+      <c r="J22" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="61"/>
-      <c r="L22" s="42" t="str">
-        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O10,13,0)</f>
-        <v>It is required to verify the information, when displaying the stored data</v>
-      </c>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="44"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="55" t="str">
+        <f>VLOOKUP(C10,'Product Backlog- HU'!B6:O9,13,0)</f>
+        <v>It is required to verify that the information, has been remove the database</v>
+      </c>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="57"/>
       <c r="P22" s="21"/>
     </row>
     <row r="23" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="17"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="47"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="60"/>
       <c r="I23" s="20"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="66"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="47"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="60"/>
       <c r="P23" s="21"/>
     </row>
     <row r="24" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="17"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="63"/>
       <c r="I24" s="20"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="63"/>
       <c r="P24" s="21"/>
     </row>
     <row r="25" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5106,6 +5041,11 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="M15:O17"/>
+    <mergeCell ref="E19:O20"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C19:D20"/>
     <mergeCell ref="C22:D24"/>
@@ -5122,11 +5062,6 @@
     <mergeCell ref="D15:E17"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H15:J17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="M15:O17"/>
-    <mergeCell ref="E19:O20"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
@@ -5157,7 +5092,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
-            <xm:f>'Product Backlog- HU'!$B$6:$B$10</xm:f>
+            <xm:f>'Product Backlog- HU'!$B$6:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>C10:C11</xm:sqref>
         </x14:dataValidation>

</xml_diff>